<commit_message>
Renumbered the paths in Excel from 0 and fixed the original python code
</commit_message>
<xml_diff>
--- a/3- LSMC/3.1-Original_example/3.1.1-Original_Excel.xlsx
+++ b/3- LSMC/3.1-Original_example/3.1.1-Original_Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p_h_d\Dropbox\2-TEACHING\000 - LSMC\SUPER_LSMC\fundamental\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p_h_d\Dropbox\2-TEACHING\000 - LSMC\SUPER_LSMC\3- LSMC\3.1-Original_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97348F2B-BAB3-4636-905B-32B4F892ECDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C507F11E-B8BD-4F0E-8BE0-AF7746FC4D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1F1D4625-D39B-4428-A9DE-637A78BF9F19}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1F1D4625-D39B-4428-A9DE-637A78BF9F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -2180,8 +2180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A6D6C7D-5047-4D1E-8F63-F2CFB597204C}">
   <dimension ref="A1:Z100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91:A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2521,7 +2521,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B37" s="5">
         <f t="shared" ref="B37:D44" si="1">MAX(0,STRIKE-B11)</f>
@@ -2545,7 +2545,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B38" s="5">
         <f t="shared" si="1"/>
@@ -2569,7 +2569,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B39" s="5">
         <f t="shared" si="1"/>
@@ -2593,7 +2593,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B40" s="5">
         <f t="shared" si="1"/>
@@ -2617,7 +2617,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B41" s="5">
         <f t="shared" si="1"/>
@@ -2641,7 +2641,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B42" s="5">
         <f t="shared" si="1"/>
@@ -2665,7 +2665,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B43" s="5">
         <f t="shared" si="1"/>
@@ -2689,7 +2689,7 @@
     </row>
     <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B44" s="5">
         <f t="shared" si="1"/>
@@ -2879,7 +2879,7 @@
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D60" s="9" cm="1">
         <f t="array" ref="D60:D67">EXP(-RISKFREE*1)*payoff_t3</f>
@@ -2902,7 +2902,7 @@
       </c>
       <c r="L60" s="4" cm="1">
         <f t="array" ref="L60:L64">_xlfn._xlws.FILTER(A60:A67,F60:F67)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M60" cm="1">
         <f t="array" ref="M60:M64">_xlfn._xlws.FILTER(H60:H67,F60:F67)</f>
@@ -2943,7 +2943,7 @@
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D61" s="9">
         <v>0</v>
@@ -2961,7 +2961,7 @@
         <v>1.5876000000000001</v>
       </c>
       <c r="L61" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M61">
         <v>1</v>
@@ -2996,7 +2996,7 @@
     </row>
     <row r="62" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D62" s="9">
         <v>6.5923517350897465E-2</v>
@@ -3014,7 +3014,7 @@
         <v>1.1449</v>
       </c>
       <c r="L62" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M62">
         <v>1</v>
@@ -3049,7 +3049,7 @@
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D63" s="9">
         <v>0.16951761604516483</v>
@@ -3067,7 +3067,7 @@
         <v>0.94089999999999996</v>
       </c>
       <c r="L63" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M63">
         <v>1</v>
@@ -3099,7 +3099,7 @@
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D64" s="9">
         <v>0</v>
@@ -3117,7 +3117,7 @@
         <v>2.4336000000000002</v>
       </c>
       <c r="L64" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M64">
         <v>1</v>
@@ -3149,7 +3149,7 @@
     </row>
     <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D65" s="9">
         <v>0.18835290671684982</v>
@@ -3173,7 +3173,7 @@
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D66" s="9">
         <v>8.4758808022582455E-2</v>
@@ -3197,7 +3197,7 @@
     </row>
     <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D67" s="9">
         <v>0</v>
@@ -3326,7 +3326,7 @@
     </row>
     <row r="75" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C75" s="9">
         <f t="shared" ref="C75:C82" si="4">EXP(-RISKFREE*(Z60-$B$72))*IF(Z60=3,E37,D37)</f>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="L75" s="4" cm="1">
         <f t="array" ref="L75:L79">_xlfn._xlws.FILTER(A75:A82,F75:F82)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M75" cm="1">
         <f t="array" ref="M75:M79">_xlfn._xlws.FILTER(H75:H82,F75:F82)</f>
@@ -3390,7 +3390,7 @@
     </row>
     <row r="76" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C76" s="9">
         <f t="shared" si="4"/>
@@ -3409,7 +3409,7 @@
         <v>1.3455999999999999</v>
       </c>
       <c r="L76" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M76">
         <v>1</v>
@@ -3443,7 +3443,7 @@
     </row>
     <row r="77" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C77" s="9">
         <f t="shared" si="4"/>
@@ -3462,7 +3462,7 @@
         <v>1.4883999999999999</v>
       </c>
       <c r="L77" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M77">
         <v>1</v>
@@ -3496,7 +3496,7 @@
     </row>
     <row r="78" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C78" s="9">
         <f t="shared" si="4"/>
@@ -3515,7 +3515,7 @@
         <v>0.86490000000000011</v>
       </c>
       <c r="L78" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M78">
         <v>1</v>
@@ -3546,7 +3546,7 @@
     </row>
     <row r="79" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C79" s="9">
         <f t="shared" si="4"/>
@@ -3565,7 +3565,7 @@
         <v>1.2321000000000002</v>
       </c>
       <c r="L79" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M79">
         <v>1</v>
@@ -3596,7 +3596,7 @@
     </row>
     <row r="80" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C80" s="9">
         <f t="shared" si="4"/>
@@ -3621,7 +3621,7 @@
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C81" s="9">
         <f t="shared" si="4"/>
@@ -3646,7 +3646,7 @@
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C82" s="9">
         <f t="shared" si="4"/>
@@ -3710,7 +3710,7 @@
     </row>
     <row r="91" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B91" s="9">
         <f t="shared" ref="B91:B98" si="6">EXP(-RISKFREE*(Z75-$B$88))*IF(Z75=3,E37,IF(Z75=2,D37,C37))</f>
@@ -3719,7 +3719,7 @@
     </row>
     <row r="92" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B92" s="9">
         <f t="shared" si="6"/>
@@ -3728,7 +3728,7 @@
     </row>
     <row r="93" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B93" s="9">
         <f t="shared" si="6"/>
@@ -3737,7 +3737,7 @@
     </row>
     <row r="94" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B94" s="9">
         <f t="shared" si="6"/>
@@ -3746,7 +3746,7 @@
     </row>
     <row r="95" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B95" s="9">
         <f t="shared" si="6"/>
@@ -3755,7 +3755,7 @@
     </row>
     <row r="96" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B96" s="9">
         <f t="shared" si="6"/>
@@ -3764,7 +3764,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B97" s="9">
         <f t="shared" si="6"/>
@@ -3773,7 +3773,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B98" s="9">
         <f t="shared" si="6"/>

</xml_diff>